<commit_message>
Create supplier should allow only saving of details
</commit_message>
<xml_diff>
--- a/Admin/Suppliers/Manual testcases/Supplier lising page.xlsx
+++ b/Admin/Suppliers/Manual testcases/Supplier lising page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Suppliers\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514FA0D1-2326-4AA1-9E79-65E64662F065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C4D4CF-A235-425A-BFFE-2ABA251E6722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,22 +113,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">It shows Company details </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Checkbox of Active, Company market dropdown, Company name, Also known as, Company Reg.No, Address, Logo, Supplier email, Supplier Phone, Short description, Long description, Company time zone, Subscription information, Send subscription related notifications to, Pricing, Inventory, Email upcoming delivery schedule to, Payments, Notifications, Activity reports, Cancel and Save changes and Create user"</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Once click the suppliers menu it should display 2 tabs they are</t>
     </r>
     <r>
@@ -205,6 +189,22 @@
   </si>
   <si>
     <t>Currently we do not have the “GST/tax registration number” field for suppliers, only buyer companies</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It shows Company details </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Checkbox of Active, Company market dropdown, Company name, Also known as, Company Reg.No, Address, Logo, Supplier email, Supplier Phone, Short description, Long description, Company time zone, Subscription information, Send subscription related notifications to, Pricing, Inventory, Email upcoming delivery schedule to, Payments, Notifications, Activity reports, Cancel , Save supplier only and Save supplier and Create new user"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>21</v>
@@ -757,10 +757,10 @@
         <v>22</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>12</v>
@@ -777,13 +777,13 @@
         <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>12</v>

</xml_diff>